<commit_message>
Fixed thermal storage calculation and updated Conversion data
</commit_message>
<xml_diff>
--- a/cea/databases/SG/components/CONVERSION.xlsx
+++ b/cea/databases/SG/components/CONVERSION.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\CityEnergyAnalyst\CityEnergyAnalyst\CityEnergyAnalyst\cea\databases\SG\components\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gnappi\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F588638B-AE05-42C8-B34F-7023C4550399}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4607AAD1-083A-46EC-A7FB-AC106CC2D7D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2325" yWindow="1275" windowWidth="22125" windowHeight="11220" tabRatio="993" firstSheet="7" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5565" yWindow="0" windowWidth="22125" windowHeight="11220" tabRatio="993" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PHOTOVOLTAIC_PANELS" sheetId="1" r:id="rId1"/>
@@ -1650,8 +1650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB10"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U5" sqref="U5"/>
+    <sheetView topLeftCell="R1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U8" sqref="U8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1823,9 +1823,8 @@
       <c r="T2" s="2">
         <v>0</v>
       </c>
-      <c r="U2" s="4">
-        <f>3.5/0.962</f>
-        <v>3.6382536382536386</v>
+      <c r="U2" s="7">
+        <v>1.54</v>
       </c>
       <c r="V2" s="2">
         <v>1</v>
@@ -1910,9 +1909,9 @@
       <c r="T3" s="2">
         <v>0</v>
       </c>
-      <c r="U3" s="4">
-        <f>2.5/0.962</f>
-        <v>2.5987525987525988</v>
+      <c r="U3" s="7">
+        <f>0.94</f>
+        <v>0.94</v>
       </c>
       <c r="V3" s="2">
         <v>1</v>
@@ -1997,9 +1996,9 @@
       <c r="T4" s="2">
         <v>0</v>
       </c>
-      <c r="U4" s="4">
-        <f>2.5/0.962</f>
-        <v>2.5987525987525988</v>
+      <c r="U4" s="7">
+        <f>0.94</f>
+        <v>0.94</v>
       </c>
       <c r="V4" s="2">
         <v>1</v>
@@ -2084,9 +2083,8 @@
       <c r="T5" s="2">
         <v>0</v>
       </c>
-      <c r="U5" s="4">
-        <f>3.5/0.962</f>
-        <v>3.6382536382536386</v>
+      <c r="U5" s="7">
+        <v>1.54</v>
       </c>
       <c r="V5" s="2">
         <v>1</v>
@@ -2171,9 +2169,9 @@
       <c r="T6" s="2">
         <v>0</v>
       </c>
-      <c r="U6" s="4">
-        <f>2.5/0.962</f>
-        <v>2.5987525987525988</v>
+      <c r="U6" s="7">
+        <f>0.94</f>
+        <v>0.94</v>
       </c>
       <c r="V6" s="2">
         <v>1</v>
@@ -2258,9 +2256,9 @@
       <c r="T7" s="2">
         <v>0</v>
       </c>
-      <c r="U7" s="4">
-        <f>2.5/0.962</f>
-        <v>2.5987525987525988</v>
+      <c r="U7" s="7">
+        <f>0.94</f>
+        <v>0.94</v>
       </c>
       <c r="V7" s="2">
         <v>1</v>
@@ -2345,9 +2343,8 @@
       <c r="T8" s="2">
         <v>0</v>
       </c>
-      <c r="U8" s="4">
-        <f>3.5/0.962</f>
-        <v>3.6382536382536386</v>
+      <c r="U8" s="7">
+        <v>1.54</v>
       </c>
       <c r="V8" s="2">
         <v>1</v>
@@ -2432,9 +2429,9 @@
       <c r="T9" s="2">
         <v>0</v>
       </c>
-      <c r="U9" s="4">
-        <f>2.5/0.962</f>
-        <v>2.5987525987525988</v>
+      <c r="U9" s="7">
+        <f>0.94</f>
+        <v>0.94</v>
       </c>
       <c r="V9" s="2">
         <v>1</v>
@@ -2519,9 +2516,9 @@
       <c r="T10" s="2">
         <v>0</v>
       </c>
-      <c r="U10" s="4">
-        <f>2.5/0.962</f>
-        <v>2.5987525987525988</v>
+      <c r="U10" s="7">
+        <f>0.94</f>
+        <v>0.94</v>
       </c>
       <c r="V10" s="2">
         <v>1</v>
@@ -4246,7 +4243,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:AB7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -6213,8 +6210,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AH3"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W6" sqref="W6"/>
+    <sheetView topLeftCell="U1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AH6" sqref="AH6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6434,7 +6431,7 @@
         <v>20</v>
       </c>
       <c r="AF2" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AG2" s="2">
         <v>5</v>
@@ -6526,8 +6523,7 @@
         <v>0</v>
       </c>
       <c r="AA3" s="7">
-        <f>2.05/0.962</f>
-        <v>2.130977130977131</v>
+        <v>1.33</v>
       </c>
       <c r="AB3" s="2">
         <v>1</v>
@@ -6542,7 +6538,7 @@
         <v>20</v>
       </c>
       <c r="AF3" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="AG3" s="2">
         <v>5</v>
@@ -6563,7 +6559,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
@@ -7388,8 +7384,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:W13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:B10"/>
+    <sheetView topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="V3" sqref="V3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8549,7 +8545,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:V15"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
@@ -9070,7 +9066,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:AG7"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="T14" sqref="T14"/>
     </sheetView>
   </sheetViews>
@@ -9804,7 +9800,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:V7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="V23" sqref="V23"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Replaced Conversion database for PV conflict
In order to avoid conflict on PV installation, only one PV type is used in the optimisation
</commit_message>
<xml_diff>
--- a/cea/databases/SG/components/CONVERSION.xlsx
+++ b/cea/databases/SG/components/CONVERSION.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gnappi\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CEATesting\THESIS_TEST_CASES_RENEWABLES\Open_High_Rise\inputs\technology\components\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9CFF043-CDE7-4A40-B056-D1B371E28868}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E23BA9A1-271E-42A7-96C8-7A0FCCFD836F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1590" yWindow="2895" windowWidth="25830" windowHeight="12315" tabRatio="1000" firstSheet="6" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PHOTOVOLTAIC_PANELS" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1032" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="996" uniqueCount="265">
   <si>
     <t>Description</t>
   </si>
@@ -153,18 +153,6 @@
   </si>
   <si>
     <t>IR_%, capacity</t>
-  </si>
-  <si>
-    <t>generic polycrystalline panel</t>
-  </si>
-  <si>
-    <t>PV2</t>
-  </si>
-  <si>
-    <t>generic amorphous silicon panel</t>
-  </si>
-  <si>
-    <t>PV3</t>
   </si>
   <si>
     <t>module_area_m2</t>
@@ -1687,14 +1675,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB10"/>
+  <dimension ref="A1:AB4"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="B1" sqref="B1"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
-      <selection pane="bottomRight" activeCell="Q11" sqref="Q11"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1751,7 +1735,7 @@
         <v>9</v>
       </c>
       <c r="K1" s="36" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="L1" s="36" t="s">
         <v>10</v>
@@ -2060,522 +2044,6 @@
         <v>5</v>
       </c>
       <c r="AB4" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="2">
-        <v>1</v>
-      </c>
-      <c r="E5" s="2">
-        <v>10000</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G5" s="2">
-        <v>1</v>
-      </c>
-      <c r="H5" s="2">
-        <v>2E-3</v>
-      </c>
-      <c r="I5" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="J5" s="2">
-        <v>43.9</v>
-      </c>
-      <c r="K5" s="2">
-        <v>30</v>
-      </c>
-      <c r="L5" s="2">
-        <v>4.4000000000000003E-3</v>
-      </c>
-      <c r="M5" s="3">
-        <v>0.91809300000000005</v>
-      </c>
-      <c r="N5" s="3">
-        <v>8.6257E-2</v>
-      </c>
-      <c r="O5" s="3">
-        <v>-2.4459000000000002E-2</v>
-      </c>
-      <c r="P5" s="3">
-        <v>2.8159999999999999E-3</v>
-      </c>
-      <c r="Q5" s="3">
-        <v>-1.26E-4</v>
-      </c>
-      <c r="R5" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="S5" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="T5" s="2">
-        <v>0</v>
-      </c>
-      <c r="U5" s="7">
-        <v>0.89</v>
-      </c>
-      <c r="V5" s="2">
-        <v>1</v>
-      </c>
-      <c r="W5" s="2">
-        <v>0</v>
-      </c>
-      <c r="X5" s="2">
-        <v>0</v>
-      </c>
-      <c r="Y5" s="2">
-        <v>20</v>
-      </c>
-      <c r="Z5" s="2">
-        <v>1</v>
-      </c>
-      <c r="AA5" s="2">
-        <v>5</v>
-      </c>
-      <c r="AB5" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" s="2">
-        <v>10000</v>
-      </c>
-      <c r="E6" s="2">
-        <v>200000</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G6" s="2">
-        <v>1</v>
-      </c>
-      <c r="H6" s="2">
-        <v>2E-3</v>
-      </c>
-      <c r="I6" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="J6" s="2">
-        <v>43.9</v>
-      </c>
-      <c r="K6" s="2">
-        <v>30</v>
-      </c>
-      <c r="L6" s="2">
-        <v>4.4000000000000003E-3</v>
-      </c>
-      <c r="M6" s="3">
-        <v>0.91809300000000005</v>
-      </c>
-      <c r="N6" s="3">
-        <v>8.6257E-2</v>
-      </c>
-      <c r="O6" s="3">
-        <v>-2.4459000000000002E-2</v>
-      </c>
-      <c r="P6" s="3">
-        <v>2.8159999999999999E-3</v>
-      </c>
-      <c r="Q6" s="3">
-        <v>-1.26E-4</v>
-      </c>
-      <c r="R6" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="S6" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="T6" s="2">
-        <v>0</v>
-      </c>
-      <c r="U6" s="7">
-        <v>0.54400000000000004</v>
-      </c>
-      <c r="V6" s="2">
-        <v>1</v>
-      </c>
-      <c r="W6" s="2">
-        <v>0</v>
-      </c>
-      <c r="X6" s="2">
-        <v>0</v>
-      </c>
-      <c r="Y6" s="2">
-        <v>20</v>
-      </c>
-      <c r="Z6" s="2">
-        <v>1</v>
-      </c>
-      <c r="AA6" s="2">
-        <v>5</v>
-      </c>
-      <c r="AB6" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" s="2">
-        <v>200000</v>
-      </c>
-      <c r="E7" s="5">
-        <v>10000000000</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G7" s="2">
-        <v>1</v>
-      </c>
-      <c r="H7" s="2">
-        <v>2E-3</v>
-      </c>
-      <c r="I7" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="J7" s="2">
-        <v>43.9</v>
-      </c>
-      <c r="K7" s="2">
-        <v>30</v>
-      </c>
-      <c r="L7" s="2">
-        <v>4.4000000000000003E-3</v>
-      </c>
-      <c r="M7" s="3">
-        <v>0.91809300000000005</v>
-      </c>
-      <c r="N7" s="3">
-        <v>8.6257E-2</v>
-      </c>
-      <c r="O7" s="3">
-        <v>-2.4459000000000002E-2</v>
-      </c>
-      <c r="P7" s="3">
-        <v>2.8159999999999999E-3</v>
-      </c>
-      <c r="Q7" s="3">
-        <v>-1.26E-4</v>
-      </c>
-      <c r="R7" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="S7" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="T7" s="2">
-        <v>0</v>
-      </c>
-      <c r="U7" s="7">
-        <v>0.54400000000000004</v>
-      </c>
-      <c r="V7" s="2">
-        <v>1</v>
-      </c>
-      <c r="W7" s="2">
-        <v>0</v>
-      </c>
-      <c r="X7" s="2">
-        <v>0</v>
-      </c>
-      <c r="Y7" s="2">
-        <v>20</v>
-      </c>
-      <c r="Z7" s="2">
-        <v>1</v>
-      </c>
-      <c r="AA7" s="2">
-        <v>5</v>
-      </c>
-      <c r="AB7" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="2">
-        <v>1</v>
-      </c>
-      <c r="E8" s="2">
-        <v>10000</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G8" s="2">
-        <v>1</v>
-      </c>
-      <c r="H8" s="2">
-        <v>2E-3</v>
-      </c>
-      <c r="I8" s="2">
-        <v>0.08</v>
-      </c>
-      <c r="J8" s="2">
-        <v>38.1</v>
-      </c>
-      <c r="K8" s="2">
-        <v>30</v>
-      </c>
-      <c r="L8" s="2">
-        <v>2.5999999999999999E-3</v>
-      </c>
-      <c r="M8" s="3">
-        <v>1.10044085</v>
-      </c>
-      <c r="N8" s="3">
-        <v>-6.1423230000000002E-2</v>
-      </c>
-      <c r="O8" s="3">
-        <v>-4.4273200000000002E-3</v>
-      </c>
-      <c r="P8" s="3">
-        <v>6.3150399999999996E-4</v>
-      </c>
-      <c r="Q8" s="3">
-        <v>-1.9184000000000001E-5</v>
-      </c>
-      <c r="R8" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="S8" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="T8" s="2">
-        <v>0</v>
-      </c>
-      <c r="U8" s="7">
-        <v>0.89</v>
-      </c>
-      <c r="V8" s="2">
-        <v>1</v>
-      </c>
-      <c r="W8" s="2">
-        <v>0</v>
-      </c>
-      <c r="X8" s="2">
-        <v>0</v>
-      </c>
-      <c r="Y8" s="2">
-        <v>20</v>
-      </c>
-      <c r="Z8" s="2">
-        <v>1</v>
-      </c>
-      <c r="AA8" s="2">
-        <v>5</v>
-      </c>
-      <c r="AB8" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" s="2">
-        <v>10000</v>
-      </c>
-      <c r="E9" s="2">
-        <v>200000</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G9" s="2">
-        <v>1</v>
-      </c>
-      <c r="H9" s="2">
-        <v>2E-3</v>
-      </c>
-      <c r="I9" s="2">
-        <v>0.08</v>
-      </c>
-      <c r="J9" s="2">
-        <v>38.1</v>
-      </c>
-      <c r="K9" s="2">
-        <v>30</v>
-      </c>
-      <c r="L9" s="2">
-        <v>2.5999999999999999E-3</v>
-      </c>
-      <c r="M9" s="3">
-        <v>1.10044085</v>
-      </c>
-      <c r="N9" s="3">
-        <v>-6.1423230000000002E-2</v>
-      </c>
-      <c r="O9" s="3">
-        <v>-4.4273200000000002E-3</v>
-      </c>
-      <c r="P9" s="3">
-        <v>6.3150399999999996E-4</v>
-      </c>
-      <c r="Q9" s="3">
-        <v>-1.9184000000000001E-5</v>
-      </c>
-      <c r="R9" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="S9" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="T9" s="2">
-        <v>0</v>
-      </c>
-      <c r="U9" s="7">
-        <v>0.54400000000000004</v>
-      </c>
-      <c r="V9" s="2">
-        <v>1</v>
-      </c>
-      <c r="W9" s="2">
-        <v>0</v>
-      </c>
-      <c r="X9" s="2">
-        <v>0</v>
-      </c>
-      <c r="Y9" s="2">
-        <v>20</v>
-      </c>
-      <c r="Z9" s="2">
-        <v>1</v>
-      </c>
-      <c r="AA9" s="2">
-        <v>5</v>
-      </c>
-      <c r="AB9" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="2">
-        <v>200000</v>
-      </c>
-      <c r="E10" s="5">
-        <v>10000000000</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G10" s="2">
-        <v>1</v>
-      </c>
-      <c r="H10" s="2">
-        <v>2E-3</v>
-      </c>
-      <c r="I10" s="2">
-        <v>0.08</v>
-      </c>
-      <c r="J10" s="2">
-        <v>38.1</v>
-      </c>
-      <c r="K10" s="2">
-        <v>30</v>
-      </c>
-      <c r="L10" s="2">
-        <v>2.5999999999999999E-3</v>
-      </c>
-      <c r="M10" s="3">
-        <v>1.10044085</v>
-      </c>
-      <c r="N10" s="3">
-        <v>-6.1423230000000002E-2</v>
-      </c>
-      <c r="O10" s="3">
-        <v>-4.4273200000000002E-3</v>
-      </c>
-      <c r="P10" s="3">
-        <v>6.3150399999999996E-4</v>
-      </c>
-      <c r="Q10" s="3">
-        <v>-1.9184000000000001E-5</v>
-      </c>
-      <c r="R10" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="S10" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="T10" s="2">
-        <v>0</v>
-      </c>
-      <c r="U10" s="7">
-        <v>0.54400000000000004</v>
-      </c>
-      <c r="V10" s="2">
-        <v>1</v>
-      </c>
-      <c r="W10" s="2">
-        <v>0</v>
-      </c>
-      <c r="X10" s="2">
-        <v>0</v>
-      </c>
-      <c r="Y10" s="2">
-        <v>20</v>
-      </c>
-      <c r="Z10" s="2">
-        <v>1</v>
-      </c>
-      <c r="AA10" s="2">
-        <v>5</v>
-      </c>
-      <c r="AB10" s="2" t="s">
         <v>32</v>
       </c>
     </row>
@@ -2622,25 +2090,25 @@
         <v>5</v>
       </c>
       <c r="G1" s="36" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="H1" s="36" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="I1" s="36" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="J1" s="36" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="K1" s="36" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="L1" s="36" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="M1" s="36" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="N1" s="36" t="s">
         <v>17</v>
@@ -2673,18 +2141,18 @@
         <v>26</v>
       </c>
       <c r="X1" s="40" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D2" s="17">
         <v>1</v>
@@ -2708,13 +2176,13 @@
         <v>27</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>31</v>
@@ -2744,21 +2212,21 @@
         <v>1</v>
       </c>
       <c r="W2" s="11" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="X2" s="27" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D3" s="17">
         <v>1</v>
@@ -2782,13 +2250,13 @@
         <v>28</v>
       </c>
       <c r="K3" s="12" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="N3" s="2" t="s">
         <v>31</v>
@@ -2818,21 +2286,21 @@
         <v>1</v>
       </c>
       <c r="W3" s="11" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="X3" s="27" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D4" s="17">
         <v>1</v>
@@ -2856,13 +2324,13 @@
         <v>27</v>
       </c>
       <c r="K4" s="43" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="N4" s="2" t="s">
         <v>31</v>
@@ -2892,10 +2360,10 @@
         <v>1</v>
       </c>
       <c r="W4" s="11" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="X4" s="27" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
   </sheetData>
@@ -2937,22 +2405,22 @@
         <v>5</v>
       </c>
       <c r="G1" s="36" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="H1" s="36" t="s">
+        <v>213</v>
+      </c>
+      <c r="I1" s="36" t="s">
+        <v>215</v>
+      </c>
+      <c r="J1" s="36" t="s">
+        <v>214</v>
+      </c>
+      <c r="K1" s="36" t="s">
         <v>217</v>
       </c>
-      <c r="I1" s="36" t="s">
-        <v>219</v>
-      </c>
-      <c r="J1" s="36" t="s">
+      <c r="L1" s="36" t="s">
         <v>218</v>
-      </c>
-      <c r="K1" s="36" t="s">
-        <v>221</v>
-      </c>
-      <c r="L1" s="36" t="s">
-        <v>222</v>
       </c>
       <c r="M1" s="36" t="s">
         <v>17</v>
@@ -2985,18 +2453,18 @@
         <v>26</v>
       </c>
       <c r="W1" s="40" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="D2" s="17">
         <v>0</v>
@@ -3005,7 +2473,7 @@
         <v>100000000</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="G2" s="2">
         <v>1</v>
@@ -3020,10 +2488,10 @@
         <v>1500</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>31</v>
@@ -3053,10 +2521,10 @@
         <v>5</v>
       </c>
       <c r="V2" s="14" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="W2" s="27" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
   </sheetData>
@@ -3125,15 +2593,15 @@
         <v>25</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="C2" s="2">
         <v>1000</v>
@@ -3176,10 +2644,10 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="C3" s="2">
         <v>1</v>
@@ -3219,7 +2687,7 @@
         <v>5</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
   </sheetData>
@@ -3272,16 +2740,16 @@
         <v>5</v>
       </c>
       <c r="G1" s="36" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="H1" s="36" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="I1" s="36" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="J1" s="36" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="K1" s="36" t="s">
         <v>17</v>
@@ -3314,18 +2782,18 @@
         <v>26</v>
       </c>
       <c r="U1" s="36" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>143</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>147</v>
       </c>
       <c r="D2" s="17">
         <v>0</v>
@@ -3376,21 +2844,21 @@
         <v>5</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D3" s="17">
         <v>0</v>
@@ -3441,10 +2909,10 @@
         <v>5</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
@@ -3505,22 +2973,22 @@
         <v>5</v>
       </c>
       <c r="G1" s="40" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="H1" s="40" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="I1" s="40" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="J1" s="40" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="K1" s="40" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="L1" s="40" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="M1" s="38" t="s">
         <v>17</v>
@@ -3553,18 +3021,18 @@
         <v>26</v>
       </c>
       <c r="W1" s="40" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="D2" s="17">
         <v>0</v>
@@ -3588,10 +3056,10 @@
         <v>27</v>
       </c>
       <c r="K2" s="11" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="L2" s="11" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="M2" s="19" t="s">
         <v>31</v>
@@ -3623,18 +3091,18 @@
       </c>
       <c r="V2" s="14"/>
       <c r="W2" s="27" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="D3" s="17">
         <v>40000</v>
@@ -3658,10 +3126,10 @@
         <v>27</v>
       </c>
       <c r="K3" s="11" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="L3" s="11" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="M3" s="19" t="s">
         <v>31</v>
@@ -3693,18 +3161,18 @@
       </c>
       <c r="V3" s="14"/>
       <c r="W3" s="27" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="D4" s="17">
         <v>0</v>
@@ -3728,10 +3196,10 @@
         <v>27</v>
       </c>
       <c r="K4" s="11" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="L4" s="11" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="M4" s="19" t="s">
         <v>31</v>
@@ -3764,18 +3232,18 @@
       </c>
       <c r="V4" s="14"/>
       <c r="W4" s="27" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="D5" s="17">
         <v>21000</v>
@@ -3799,10 +3267,10 @@
         <v>27</v>
       </c>
       <c r="K5" s="11" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="L5" s="11" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="M5" s="19" t="s">
         <v>31</v>
@@ -3835,18 +3303,18 @@
       </c>
       <c r="V5" s="14"/>
       <c r="W5" s="27" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="D6" s="17">
         <v>40000</v>
@@ -3870,10 +3338,10 @@
         <v>27</v>
       </c>
       <c r="K6" s="11" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="L6" s="11" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="M6" s="19" t="s">
         <v>31</v>
@@ -3906,18 +3374,18 @@
       </c>
       <c r="V6" s="14"/>
       <c r="W6" s="27" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="D7" s="17">
         <v>75000</v>
@@ -3941,10 +3409,10 @@
         <v>27</v>
       </c>
       <c r="K7" s="11" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="L7" s="11" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="M7" s="19" t="s">
         <v>31</v>
@@ -3977,18 +3445,18 @@
       </c>
       <c r="V7" s="14"/>
       <c r="W7" s="27" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D8" s="17">
         <v>0</v>
@@ -4012,10 +3480,10 @@
         <v>35</v>
       </c>
       <c r="K8" s="11" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="L8" s="11" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="M8" s="19" t="s">
         <v>31</v>
@@ -4046,21 +3514,21 @@
         <v>6</v>
       </c>
       <c r="V8" s="14" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="W8" s="27" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D9" s="17">
         <v>21000</v>
@@ -4084,10 +3552,10 @@
         <v>35</v>
       </c>
       <c r="K9" s="11" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="L9" s="11" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="M9" s="19" t="s">
         <v>31</v>
@@ -4118,21 +3586,21 @@
         <v>6</v>
       </c>
       <c r="V9" s="14" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="W9" s="27" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D10" s="17">
         <v>40000</v>
@@ -4156,10 +3624,10 @@
         <v>35</v>
       </c>
       <c r="K10" s="11" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="L10" s="11" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="M10" s="19" t="s">
         <v>31</v>
@@ -4190,21 +3658,21 @@
         <v>6</v>
       </c>
       <c r="V10" s="14" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="W10" s="27" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D11" s="17">
         <v>75000</v>
@@ -4228,10 +3696,10 @@
         <v>35</v>
       </c>
       <c r="K11" s="11" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="L11" s="11" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="M11" s="19" t="s">
         <v>31</v>
@@ -4262,10 +3730,10 @@
         <v>6</v>
       </c>
       <c r="V11" s="14" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="W11" s="27" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
   </sheetData>
@@ -4280,7 +3748,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:AB7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -4945,13 +4413,13 @@
         <v>4</v>
       </c>
       <c r="F1" s="36" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="G1" s="36" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="H1" s="36" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="I1" s="36" t="s">
         <v>17</v>
@@ -4975,7 +4443,7 @@
         <v>23</v>
       </c>
       <c r="P1" s="36" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="Q1" s="36" t="s">
         <v>24</v>
@@ -4984,31 +4452,31 @@
         <v>25</v>
       </c>
       <c r="S1" s="36" t="s">
+        <v>94</v>
+      </c>
+      <c r="T1" s="36" t="s">
+        <v>95</v>
+      </c>
+      <c r="U1" s="36" t="s">
+        <v>96</v>
+      </c>
+      <c r="V1" s="36" t="s">
+        <v>97</v>
+      </c>
+      <c r="W1" s="36" t="s">
         <v>98</v>
       </c>
-      <c r="T1" s="36" t="s">
+      <c r="X1" s="36" t="s">
         <v>99</v>
       </c>
-      <c r="U1" s="36" t="s">
+      <c r="Y1" s="36" t="s">
         <v>100</v>
       </c>
-      <c r="V1" s="36" t="s">
+      <c r="Z1" s="36" t="s">
         <v>101</v>
       </c>
-      <c r="W1" s="36" t="s">
+      <c r="AA1" s="36" t="s">
         <v>102</v>
-      </c>
-      <c r="X1" s="36" t="s">
-        <v>103</v>
-      </c>
-      <c r="Y1" s="36" t="s">
-        <v>104</v>
-      </c>
-      <c r="Z1" s="36" t="s">
-        <v>105</v>
-      </c>
-      <c r="AA1" s="36" t="s">
-        <v>106</v>
       </c>
       <c r="AB1" s="36" t="s">
         <v>26</v>
@@ -5016,13 +4484,13 @@
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D2" s="17">
         <v>0</v>
@@ -5037,7 +4505,7 @@
         <v>0.9</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="I2" s="11" t="s">
         <v>31</v>
@@ -5097,18 +4565,18 @@
         <v>0.96</v>
       </c>
       <c r="AB2" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D3" s="17">
         <v>0</v>
@@ -5123,7 +4591,7 @@
         <v>0.9</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="I3" s="11" t="s">
         <v>31</v>
@@ -5183,18 +4651,18 @@
         <v>0.96</v>
       </c>
       <c r="AB3" s="11" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D4" s="17">
         <v>0</v>
@@ -5209,7 +4677,7 @@
         <v>0.9</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="I4" s="11" t="s">
         <v>31</v>
@@ -5269,18 +4737,18 @@
         <v>0.96</v>
       </c>
       <c r="AB4" s="11" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D5" s="17">
         <v>0</v>
@@ -5295,7 +4763,7 @@
         <v>0.9</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="I5" s="11" t="s">
         <v>31</v>
@@ -5355,18 +4823,18 @@
         <v>0.96</v>
       </c>
       <c r="AB5" s="11" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D6" s="17">
         <v>0</v>
@@ -5381,7 +4849,7 @@
         <v>0.9</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="I6" s="11" t="s">
         <v>31</v>
@@ -5441,18 +4909,18 @@
         <v>0.96</v>
       </c>
       <c r="AB6" s="11" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D7" s="17">
         <v>0</v>
@@ -5467,7 +4935,7 @@
         <v>0.9</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="I7" s="11" t="s">
         <v>31</v>
@@ -5527,7 +4995,7 @@
         <v>0.96</v>
       </c>
       <c r="AB7" s="11" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -5577,10 +5045,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="36" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="G1" s="36" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="H1" s="36" t="s">
         <v>17</v>
@@ -5604,7 +5072,7 @@
         <v>23</v>
       </c>
       <c r="O1" s="36" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="P1" s="36" t="s">
         <v>24</v>
@@ -5613,34 +5081,34 @@
         <v>25</v>
       </c>
       <c r="R1" s="36" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="S1" s="36" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="T1" s="36" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="U1" s="36" t="s">
+        <v>256</v>
+      </c>
+      <c r="V1" s="36" t="s">
+        <v>257</v>
+      </c>
+      <c r="W1" s="36" t="s">
+        <v>263</v>
+      </c>
+      <c r="X1" s="36" t="s">
+        <v>259</v>
+      </c>
+      <c r="Y1" s="36" t="s">
         <v>260</v>
       </c>
-      <c r="V1" s="36" t="s">
+      <c r="Z1" s="41" t="s">
         <v>261</v>
       </c>
-      <c r="W1" s="36" t="s">
-        <v>267</v>
-      </c>
-      <c r="X1" s="36" t="s">
-        <v>263</v>
-      </c>
-      <c r="Y1" s="36" t="s">
-        <v>264</v>
-      </c>
-      <c r="Z1" s="41" t="s">
-        <v>265</v>
-      </c>
       <c r="AA1" s="41" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="AB1" s="36" t="s">
         <v>26</v>
@@ -5648,13 +5116,13 @@
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="D2" s="17">
         <v>0</v>
@@ -5666,7 +5134,7 @@
         <v>0.87</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="H2" s="11" t="s">
         <v>31</v>
@@ -5729,7 +5197,7 @@
         <v>1250000</v>
       </c>
       <c r="AB2" s="19" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -5781,22 +5249,22 @@
         <v>5</v>
       </c>
       <c r="G1" s="36" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="H1" s="36" t="s">
+        <v>213</v>
+      </c>
+      <c r="I1" s="36" t="s">
+        <v>215</v>
+      </c>
+      <c r="J1" s="36" t="s">
+        <v>214</v>
+      </c>
+      <c r="K1" s="36" t="s">
         <v>217</v>
       </c>
-      <c r="I1" s="36" t="s">
-        <v>219</v>
-      </c>
-      <c r="J1" s="36" t="s">
+      <c r="L1" s="36" t="s">
         <v>218</v>
-      </c>
-      <c r="K1" s="36" t="s">
-        <v>221</v>
-      </c>
-      <c r="L1" s="36" t="s">
-        <v>222</v>
       </c>
       <c r="M1" s="36" t="s">
         <v>17</v>
@@ -5829,18 +5297,18 @@
         <v>26</v>
       </c>
       <c r="W1" s="40" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D2" s="17">
         <v>0</v>
@@ -5849,7 +5317,7 @@
         <v>25000</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="G2" s="2">
         <v>1</v>
@@ -5864,10 +5332,10 @@
         <v>1100</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>31</v>
@@ -5899,21 +5367,21 @@
         <v>5</v>
       </c>
       <c r="V2" s="14" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="W2" s="27" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>208</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>212</v>
       </c>
       <c r="D3" s="17">
         <v>5000</v>
@@ -5922,7 +5390,7 @@
         <v>40000000</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="G3" s="2">
         <v>1</v>
@@ -5937,10 +5405,10 @@
         <v>36000</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>31</v>
@@ -5971,21 +5439,21 @@
         <v>5</v>
       </c>
       <c r="V3" s="14" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="W3" s="27" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="D4" s="17">
         <v>5000</v>
@@ -5994,7 +5462,7 @@
         <v>100000000</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="G4" s="2">
         <v>1</v>
@@ -6009,10 +5477,10 @@
         <v>100000</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>31</v>
@@ -6044,10 +5512,10 @@
         <v>5</v>
       </c>
       <c r="V4" s="14" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="W4" s="27" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
@@ -6126,10 +5594,10 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="36" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C2" s="2">
         <v>500</v>
@@ -6174,10 +5642,10 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C3" s="2">
         <v>4000</v>
@@ -6222,10 +5690,10 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C4" s="2">
         <v>37000</v>
@@ -6270,10 +5738,10 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C5" s="2">
         <v>37000</v>
@@ -6313,7 +5781,7 @@
         <v>6</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -6390,10 +5858,10 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
@@ -6478,55 +5946,55 @@
         <v>6</v>
       </c>
       <c r="E1" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="39" t="s">
+        <v>249</v>
+      </c>
+      <c r="G1" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="39" t="s">
-        <v>253</v>
-      </c>
-      <c r="G1" s="36" t="s">
+      <c r="K1" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="H1" s="36" t="s">
+      <c r="L1" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="I1" s="36" t="s">
+      <c r="M1" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="J1" s="36" t="s">
+      <c r="N1" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="K1" s="36" t="s">
+      <c r="O1" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="L1" s="36" t="s">
+      <c r="P1" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="M1" s="36" t="s">
+      <c r="Q1" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="N1" s="41" t="s">
+      <c r="R1" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="O1" s="39" t="s">
+      <c r="S1" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="P1" s="39" t="s">
+      <c r="T1" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="Q1" s="39" t="s">
+      <c r="U1" s="39" t="s">
         <v>48</v>
-      </c>
-      <c r="R1" s="39" t="s">
-        <v>49</v>
-      </c>
-      <c r="S1" s="39" t="s">
-        <v>50</v>
-      </c>
-      <c r="T1" s="39" t="s">
-        <v>51</v>
-      </c>
-      <c r="U1" s="39" t="s">
-        <v>52</v>
       </c>
       <c r="V1" s="36" t="s">
         <v>3</v>
@@ -6570,13 +6038,13 @@
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D2" s="2">
         <v>2</v>
@@ -6642,7 +6110,7 @@
         <v>10000000000</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="Y2" s="2" t="s">
         <v>31</v>
@@ -6678,13 +6146,13 @@
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D3" s="2">
         <v>2</v>
@@ -6750,7 +6218,7 @@
         <v>10000000000</v>
       </c>
       <c r="X3" s="2" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="Y3" s="2" t="s">
         <v>31</v>
@@ -6856,10 +6324,10 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
@@ -6939,7 +6407,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -6951,16 +6419,16 @@
         <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>17</v>
@@ -6993,21 +6461,21 @@
         <v>26</v>
       </c>
       <c r="V1" s="16" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>156</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>160</v>
       </c>
       <c r="E2" s="17">
         <v>1</v>
@@ -7061,21 +6529,21 @@
       </c>
       <c r="U2" s="2"/>
       <c r="V2" s="11" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>156</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>160</v>
       </c>
       <c r="E3" s="17">
         <v>90000</v>
@@ -7129,21 +6597,21 @@
       </c>
       <c r="U3" s="2"/>
       <c r="V3" s="11" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>156</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>160</v>
       </c>
       <c r="E4" s="17">
         <v>730000</v>
@@ -7197,21 +6665,21 @@
       </c>
       <c r="U4" s="2"/>
       <c r="V4" s="11" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="E5" s="17">
         <v>1</v>
@@ -7265,21 +6733,21 @@
       </c>
       <c r="U5" s="2"/>
       <c r="V5" s="11" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="E6" s="17">
         <v>90000</v>
@@ -7333,21 +6801,21 @@
       </c>
       <c r="U6" s="2"/>
       <c r="V6" s="11" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="E7" s="17">
         <v>730000</v>
@@ -7401,21 +6869,21 @@
       </c>
       <c r="U7" s="2"/>
       <c r="V7" s="11" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="E8" s="17">
         <v>1</v>
@@ -7469,21 +6937,21 @@
       </c>
       <c r="U8" s="2"/>
       <c r="V8" s="11" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="E9" s="17">
         <v>90000</v>
@@ -7537,21 +7005,21 @@
       </c>
       <c r="U9" s="2"/>
       <c r="V9" s="11" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="E10" s="17">
         <v>730000</v>
@@ -7605,7 +7073,7 @@
       </c>
       <c r="U10" s="2"/>
       <c r="V10" s="11" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -7648,7 +7116,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="36" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="E1" s="36" t="s">
         <v>3</v>
@@ -7660,19 +7128,19 @@
         <v>5</v>
       </c>
       <c r="H1" s="39" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="I1" s="39" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="J1" s="39" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="K1" s="39" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="L1" s="36" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="M1" s="36" t="s">
         <v>17</v>
@@ -7705,21 +7173,21 @@
         <v>26</v>
       </c>
       <c r="W1" s="36" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="E2" s="17">
         <v>850000</v>
@@ -7773,24 +7241,24 @@
         <v>5</v>
       </c>
       <c r="V2" s="12" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="W2" s="31" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="3" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="E3" s="17">
         <v>2600000</v>
@@ -7844,24 +7312,24 @@
         <v>5</v>
       </c>
       <c r="V3" s="12" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="W3" s="31" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="4" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="E4" s="24">
         <v>3500000</v>
@@ -7915,24 +7383,24 @@
         <v>5</v>
       </c>
       <c r="V4" s="11" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="W4" s="31" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="5" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="E5" s="25">
         <v>180000</v>
@@ -7986,24 +7454,24 @@
         <v>5</v>
       </c>
       <c r="V5" s="11" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="W5" s="31" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="6" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="E6" s="25">
         <v>280000</v>
@@ -8057,24 +7525,24 @@
         <v>5</v>
       </c>
       <c r="V6" s="11" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="W6" s="31" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="7" spans="1:23" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="E7" s="25">
         <v>900000</v>
@@ -8128,24 +7596,24 @@
         <v>5</v>
       </c>
       <c r="V7" s="11" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="W7" s="31" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="E8" s="25">
         <v>1000000</v>
@@ -8199,24 +7667,24 @@
         <v>5</v>
       </c>
       <c r="V8" s="11" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="W8" s="27" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="E9" s="25">
         <v>5000000</v>
@@ -8270,24 +7738,24 @@
         <v>5</v>
       </c>
       <c r="V9" s="11" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="W9" s="27" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="E10" s="25">
         <v>1000000</v>
@@ -8341,24 +7809,24 @@
         <v>5</v>
       </c>
       <c r="V10" s="11" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="W10" s="27" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="E11" s="25">
         <v>30000000</v>
@@ -8413,10 +7881,10 @@
         <v>6</v>
       </c>
       <c r="V11" s="11" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="W11" s="27" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
@@ -8470,16 +7938,16 @@
         <v>5</v>
       </c>
       <c r="G1" s="36" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="H1" s="36" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="I1" s="36" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="J1" s="36" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="K1" s="36" t="s">
         <v>17</v>
@@ -8512,18 +7980,18 @@
         <v>26</v>
       </c>
       <c r="U1" s="40" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D2" s="17">
         <v>1</v>
@@ -8541,10 +8009,10 @@
         <v>160</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>31</v>
@@ -8576,21 +8044,21 @@
         <v>5</v>
       </c>
       <c r="T2" s="11" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="U2" s="27" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D3" s="17">
         <v>80000</v>
@@ -8608,10 +8076,10 @@
         <v>160</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>31</v>
@@ -8642,21 +8110,21 @@
         <v>5</v>
       </c>
       <c r="T3" s="11" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="U3" s="27" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D4" s="24">
         <v>100000</v>
@@ -8674,10 +8142,10 @@
         <v>160</v>
       </c>
       <c r="I4" s="12" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="J4" s="12" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>31</v>
@@ -8709,21 +8177,21 @@
         <v>5</v>
       </c>
       <c r="T4" s="11" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="U4" s="27" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="D5" s="2">
         <v>0</v>
@@ -8732,7 +8200,7 @@
         <v>500</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
@@ -8766,7 +8234,7 @@
         <v>5</v>
       </c>
       <c r="T5" s="2" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -8807,7 +8275,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="D1" s="36" t="s">
         <v>2</v>
@@ -8822,16 +8290,16 @@
         <v>5</v>
       </c>
       <c r="H1" s="36" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="I1" s="36" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="J1" s="36" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="K1" s="36" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="L1" s="36" t="s">
         <v>17</v>
@@ -8864,21 +8332,21 @@
         <v>26</v>
       </c>
       <c r="V1" s="36" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C2" s="12">
         <v>0.47</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E2" s="17">
         <v>1050000</v>
@@ -8929,24 +8397,24 @@
         <v>5</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C3" s="11">
         <v>0.4</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E3" s="17">
         <v>1</v>
@@ -9002,21 +8470,21 @@
         <v>25</v>
       </c>
       <c r="V3" s="2" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:22" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C4" s="11">
         <v>0.4</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E4" s="17">
         <v>260000</v>
@@ -9072,21 +8540,21 @@
         <v>25</v>
       </c>
       <c r="V4" s="2" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:22" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C5" s="11">
         <v>0.4</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E5" s="17">
         <v>530000</v>
@@ -9142,21 +8610,21 @@
         <v>25</v>
       </c>
       <c r="V5" s="2" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:22" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C6" s="11">
         <v>0.4</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E6" s="17">
         <v>1050000</v>
@@ -9212,21 +8680,21 @@
         <v>25</v>
       </c>
       <c r="V6" s="2" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:22" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C7" s="11">
         <v>0.4</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E7" s="17">
         <v>2110000</v>
@@ -9281,7 +8749,7 @@
         <v>25</v>
       </c>
       <c r="V7" s="2" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
@@ -9339,22 +8807,22 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>17</v>
@@ -9387,48 +8855,48 @@
         <v>26</v>
       </c>
       <c r="W1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AC1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>74</v>
-      </c>
       <c r="AG1" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D2" s="17">
         <v>0</v>
@@ -9518,18 +8986,18 @@
         <v>2.14</v>
       </c>
       <c r="AG2" s="2" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D3" s="17">
         <v>51150</v>
@@ -9619,18 +9087,18 @@
         <v>33</v>
       </c>
       <c r="AG3" s="2" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D4" s="17">
         <v>0</v>
@@ -9720,18 +9188,18 @@
         <v>2.5</v>
       </c>
       <c r="AG4" s="2" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D5" s="17">
         <v>58150</v>
@@ -9821,18 +9289,18 @@
         <v>14</v>
       </c>
       <c r="AG5" s="2" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D6" s="17">
         <v>1337450</v>
@@ -9922,18 +9390,18 @@
         <v>431</v>
       </c>
       <c r="AG6" s="2" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D7" s="17">
         <v>116300</v>
@@ -10076,19 +9544,19 @@
         <v>5</v>
       </c>
       <c r="G1" s="36" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="H1" s="36" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="I1" s="36" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="J1" s="36" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="K1" s="36" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="L1" s="36" t="s">
         <v>17</v>
@@ -10121,18 +9589,18 @@
         <v>26</v>
       </c>
       <c r="V1" s="40" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D2" s="17">
         <v>1</v>
@@ -10186,21 +9654,21 @@
         <v>15</v>
       </c>
       <c r="U2" s="14" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="V2" s="11" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D3" s="17">
         <v>10000000</v>
@@ -10254,21 +9722,21 @@
         <v>15</v>
       </c>
       <c r="U3" s="14" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="V3" s="11" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D4" s="17">
         <v>1</v>
@@ -10325,18 +9793,18 @@
         <v>24</v>
       </c>
       <c r="V4" s="11" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D5" s="17">
         <v>10000000</v>
@@ -10390,10 +9858,10 @@
         <v>15</v>
       </c>
       <c r="U5" s="14" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="V5" s="11" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">

</xml_diff>